<commit_message>
Mapeo de objetos y ajuste para question de mensajes  generica
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/recordarusuario/recordar_usuario.xlsx
+++ b/SVP/src/test/resources/datadriven/recordarusuario/recordar_usuario.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/ProyectosTODO1/svp-rediseno-personas-web-tests-bdd-screenplay/SVP/src/test/resources/datadriven/recordarusuario/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Todo1\Automatizacion\svp-rediseno-personas-web-tests-bdd-screenplay\SVP\src\test\resources\datadriven\recordarusuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,18 +17,18 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Orientacion</t>
   </si>
@@ -73,13 +73,25 @@
   </si>
   <si>
     <t>Alterno</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>prueba</t>
+  </si>
+  <si>
+    <t>mensajeRespuesta</t>
+  </si>
+  <si>
+    <t>El usuario ha sido enviado al correo electronico</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,7 +125,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -136,11 +148,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -153,6 +176,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,27 +493,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -518,8 +545,11 @@
       <c r="J1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="K1" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -529,13 +559,24 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="F2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1234</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1234</v>
+      </c>
       <c r="J2" s="4"/>
+      <c r="K2" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -550,6 +591,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -575,19 +617,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
ajustes de Datadriven con mensajes de respuesta
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/recordarusuario/recordar_usuario.xlsx
+++ b/SVP/src/test/resources/datadriven/recordarusuario/recordar_usuario.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Orientacion</t>
   </si>
@@ -85,13 +85,16 @@
   </si>
   <si>
     <t>El usuario ha sido enviado al correo electronico</t>
+  </si>
+  <si>
+    <t>¡Lo Sentimos!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +106,14 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Mic Shell Dlg"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -163,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -179,6 +190,7 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="F3" sqref="F3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -586,12 +598,25 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="F3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1234</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1234</v>
+      </c>
       <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
+      <c r="K3" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="K4" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ajuste de mensajes y casos con base a diccionario funcional
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/recordarusuario/recordar_usuario.xlsx
+++ b/SVP/src/test/resources/datadriven/recordarusuario/recordar_usuario.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
     <sheet name="Listas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Orientacion</t>
   </si>
@@ -84,17 +84,26 @@
     <t>mensajeRespuesta</t>
   </si>
   <si>
-    <t>El usuario ha sido enviado al correo electronico</t>
-  </si>
-  <si>
     <t>¡Lo Sentimos!</t>
+  </si>
+  <si>
+    <t>El usuario ha sido enviado al correo electrónico</t>
+  </si>
+  <si>
+    <t>Usuario o clave inválida. Inténtalo nuevamente</t>
+  </si>
+  <si>
+    <t>La clave que usas en el cajero está bloqueada. Debes activarla en la Sucursal Física. Para mayor información comunícate con la Sucursal Telefónica.</t>
+  </si>
+  <si>
+    <t>En este momento el sistema no está disponible. Estamos trabajando para brindarte una solución.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,14 +115,6 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Mic Shell Dlg"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -174,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -190,7 +191,12 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:I3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -523,7 +529,7 @@
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="132.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -585,7 +591,7 @@
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -612,11 +618,92 @@
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="K4" s="7"/>
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1234</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1234</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1234</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1234</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="10">
+        <v>1234</v>
+      </c>
+      <c r="I6" s="10">
+        <v>1234</v>
+      </c>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="11:11">
+      <c r="K17" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -628,7 +715,7 @@
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B3</xm:sqref>
+          <xm:sqref>B2:B6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Ajustes a flujo de recordar usuario
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/recordarusuario/recordar_usuario.xlsx
+++ b/SVP/src/test/resources/datadriven/recordarusuario/recordar_usuario.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Orientacion</t>
   </si>
@@ -75,28 +75,55 @@
     <t>Alterno</t>
   </si>
   <si>
-    <t>123456789</t>
-  </si>
-  <si>
-    <t>prueba</t>
-  </si>
-  <si>
     <t>mensajeRespuesta</t>
   </si>
   <si>
     <t>¡Lo Sentimos!</t>
   </si>
   <si>
-    <t>El usuario ha sido enviado al correo electrónico</t>
-  </si>
-  <si>
     <t>Usuario o clave inválida. Inténtalo nuevamente</t>
   </si>
   <si>
-    <t>La clave que usas en el cajero está bloqueada. Debes activarla en la Sucursal Física. Para mayor información comunícate con la Sucursal Telefónica.</t>
-  </si>
-  <si>
     <t>En este momento el sistema no está disponible. Estamos trabajando para brindarte una solución.</t>
+  </si>
+  <si>
+    <t>25130110</t>
+  </si>
+  <si>
+    <t>25130111</t>
+  </si>
+  <si>
+    <t>25130112</t>
+  </si>
+  <si>
+    <t>25130114</t>
+  </si>
+  <si>
+    <t>USUCTDC1</t>
+  </si>
+  <si>
+    <t>USUCTDC2</t>
+  </si>
+  <si>
+    <t>USUCTDC3</t>
+  </si>
+  <si>
+    <t>USUCTDC5</t>
+  </si>
+  <si>
+    <t>El usuario ha sido enviado al correo electrónico.</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1989636240</t>
+  </si>
+  <si>
+    <t>OSVPPRU16</t>
+  </si>
+  <si>
+    <t>La clave que usas en el cajero está bloqueada.</t>
   </si>
 </sst>
 </file>
@@ -175,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -195,7 +222,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -514,7 +540,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -564,7 +590,7 @@
         <v>2</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -578,10 +604,10 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1">
         <v>1234</v>
@@ -591,7 +617,7 @@
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -605,25 +631,25 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H3" s="1">
-        <v>1234</v>
+        <v>4321</v>
       </c>
       <c r="I3" s="1">
         <v>1234</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="4">
-        <v>3</v>
+      <c r="A4" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -632,10 +658,10 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="H4" s="1">
         <v>1234</v>
@@ -645,7 +671,7 @@
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -659,10 +685,10 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="H5" s="1">
         <v>1234</v>
@@ -672,7 +698,7 @@
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -685,21 +711,21 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="10">
-        <v>1234</v>
-      </c>
-      <c r="I6" s="10">
+      <c r="F6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="9">
+        <v>1234</v>
+      </c>
+      <c r="I6" s="9">
         <v>1234</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="11:11">
@@ -715,7 +741,7 @@
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B6</xm:sqref>
+          <xm:sqref>B2:B4 B5:B6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
ajustes a escenario de recordar usuario maximo de intentos fallidos
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/recordarusuario/recordar_usuario.xlsx
+++ b/SVP/src/test/resources/datadriven/recordarusuario/recordar_usuario.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Orientacion</t>
   </si>
@@ -78,9 +78,6 @@
     <t>mensajeRespuesta</t>
   </si>
   <si>
-    <t>¡Lo Sentimos!</t>
-  </si>
-  <si>
     <t>Usuario o clave inválida. Inténtalo nuevamente</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>25130110</t>
   </si>
   <si>
-    <t>25130111</t>
-  </si>
-  <si>
     <t>25130112</t>
   </si>
   <si>
@@ -102,9 +96,6 @@
     <t>USUCTDC1</t>
   </si>
   <si>
-    <t>USUCTDC2</t>
-  </si>
-  <si>
     <t>USUCTDC3</t>
   </si>
   <si>
@@ -124,13 +115,19 @@
   </si>
   <si>
     <t>La clave que usas en el cajero está bloqueada.</t>
+  </si>
+  <si>
+    <t>¡Lo sentimos!</t>
+  </si>
+  <si>
+    <t>25130233</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +139,14 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Mic Shell Dlg"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -202,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -223,6 +228,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -598,7 +605,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -607,17 +614,17 @@
         <v>19</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" s="1">
-        <v>1234</v>
+        <v>4321</v>
       </c>
       <c r="I2" s="1">
         <v>1234</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -625,31 +632,31 @@
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="H3" s="1">
-        <v>4321</v>
+        <v>1234</v>
       </c>
       <c r="I3" s="1">
         <v>1234</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -658,20 +665,20 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>24</v>
+        <v>30</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="H4" s="1">
-        <v>1234</v>
+        <v>4321</v>
       </c>
       <c r="I4" s="1">
         <v>1234</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -685,10 +692,10 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H5" s="1">
         <v>1234</v>
@@ -698,7 +705,7 @@
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -712,10 +719,10 @@
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H6" s="9">
         <v>1234</v>
@@ -725,8 +732,12 @@
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8" t="s">
-        <v>18</v>
-      </c>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="G11" s="10"/>
+      <c r="K11" s="10"/>
     </row>
     <row r="17" spans="11:11">
       <c r="K17" s="7"/>
@@ -741,7 +752,7 @@
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B4 B5:B6</xm:sqref>
+          <xm:sqref>B2:B3 B4:B6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Creacion caso prueba usuario inexistente
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/recordarusuario/recordar_usuario.xlsx
+++ b/SVP/src/test/resources/datadriven/recordarusuario/recordar_usuario.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Orientacion</t>
   </si>
@@ -81,27 +81,18 @@
     <t>Usuario o clave inválida. Inténtalo nuevamente</t>
   </si>
   <si>
-    <t>En este momento el sistema no está disponible. Estamos trabajando para brindarte una solución.</t>
-  </si>
-  <si>
     <t>25130110</t>
   </si>
   <si>
     <t>25130112</t>
   </si>
   <si>
-    <t>25130114</t>
-  </si>
-  <si>
     <t>USUCTDC1</t>
   </si>
   <si>
     <t>USUCTDC3</t>
   </si>
   <si>
-    <t>USUCTDC5</t>
-  </si>
-  <si>
     <t>El usuario ha sido enviado al correo electrónico.</t>
   </si>
   <si>
@@ -120,7 +111,13 @@
     <t>¡Lo sentimos!</t>
   </si>
   <si>
-    <t>25130233</t>
+    <t>1152207037</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -207,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -224,10 +221,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -546,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -611,10 +604,10 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H2" s="1">
         <v>4321</v>
@@ -632,16 +625,16 @@
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="5" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="1">
         <v>1234</v>
@@ -651,39 +644,39 @@
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="H4" s="1">
-        <v>4321</v>
+        <v>1234</v>
       </c>
       <c r="I4" s="1">
         <v>1234</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="4">
-        <v>4</v>
+      <c r="A5" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>14</v>
@@ -692,52 +685,52 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="H5" s="1">
-        <v>1234</v>
+        <v>4321</v>
       </c>
       <c r="I5" s="1">
         <v>1234</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="8">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="9">
+        <v>24</v>
+      </c>
+      <c r="H6" s="1">
         <v>1234</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="1">
         <v>1234</v>
       </c>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8" t="s">
-        <v>17</v>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="G11" s="10"/>
-      <c r="K11" s="10"/>
+      <c r="G11" s="8"/>
+      <c r="K11" s="8"/>
     </row>
     <row r="17" spans="11:11">
       <c r="K17" s="7"/>
@@ -752,7 +745,7 @@
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B3 B4:B6</xm:sqref>
+          <xm:sqref>B2:B6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>